<commit_message>
fix wrong matrix size in 1d model
</commit_message>
<xml_diff>
--- a/cpac-data.xlsx
+++ b/cpac-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CPAC-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MultiModularity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A123BB18-90DC-48F6-8C2F-DC5F4D6BF34F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EF16C8-F231-4035-A89A-8409A32F6BA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="4650" activeTab="3" xr2:uid="{841CE58D-BA72-42A6-96EB-281E7D9E4954}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="14370" windowHeight="4650" activeTab="3" xr2:uid="{841CE58D-BA72-42A6-96EB-281E7D9E4954}"/>
   </bookViews>
   <sheets>
     <sheet name="Cross Modality" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="259">
   <si>
     <t>1.75 (0.51)</t>
   </si>
@@ -3719,6 +3719,12 @@
     <t>16样本学习</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Train Losses</t>
+  </si>
+  <si>
+    <t>Test Losses</t>
+  </si>
 </sst>
 </file>
 
@@ -5928,6 +5934,683 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>train!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Train Losses</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>train!$J$2:$J$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="58"/>
+                <c:pt idx="0">
+                  <c:v>17008.357</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17008.357</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14161.092000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14103.118</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14036.084999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17533.687000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14550.880999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14442.607</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14359.975</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14352.181</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14355.665000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14352.77</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14343.445</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14324.89</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14323.895</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14305.71</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14328.205</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>14346.89</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14311.24</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14354.678</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14350.985000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14333.406999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>14323.518</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>14366.231</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>14311.763999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>14310.839</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14356.501</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14364.191999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14295.773999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14345.221</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>14330.42</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>14342.254000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>14347.834999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>14371.05</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>14346.045</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>14329.776</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>14357.947</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>14319.233</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>14324.21</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>14338.620999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>14359.984</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>14328.364</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>14335.414000000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>14363.214</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>14335.397999999999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>14354.882</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>14328.598</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>14343.97</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>14338.165000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>14337.576999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>14365.184999999999</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>14367.597</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>14349.745999999999</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>14323.002</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>14368.772999999999</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>14379.208000000001</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>14364.629000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6BCE-45FB-9442-F771366312D7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>train!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test Losses</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>train!$K$2:$K$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="58"/>
+                <c:pt idx="0">
+                  <c:v>6576.723</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6576.723</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6359.6170000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6397.125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6367.8289999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6823.0739999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6361.7079999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6382.0640000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6878.5410000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7486.1480000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6651.9219999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6371.2550000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7285.5349999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7074.08</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7392.4870000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7179.8469999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7235</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6876.5959999999995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6936.0590000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7358.3540000000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7432.9210000000003</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7577.942</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7196.3890000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7612.91</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7526.3580000000002</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7057.5540000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7526.0140000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7690.7139999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7817.652</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7071.1419999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6947.5169999999998</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7341.7830000000004</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7651.1719999999996</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7440.4610000000002</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7665.1419999999998</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7113.6210000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6855.1970000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7865.9110000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7765.1120000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7216.8320000000003</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7376.0510000000004</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>7636.0349999999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7964.1319999999996</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7972.9549999999999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>7660.7330000000002</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7428.7669999999998</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>6663.5420000000004</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>7677.2169999999996</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>7160.37</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>7375.1210000000001</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>7095.183</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>7485.6679999999997</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>7416.6549999999997</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>6728.94</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>6987.2730000000001</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>7320.6679999999997</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>7192.5320000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6BCE-45FB-9442-F771366312D7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="413938256"/>
+        <c:axId val="416104000"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="413938256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="416104000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="416104000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="413938256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -7332,7 +8015,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -7811,7 +8494,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -9825,7 +10508,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -18267,6 +18950,46 @@
 </file>
 
 <file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -20691,6 +21414,522 @@
 </file>
 
 <file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -25670,6 +26909,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18030BC2-9E72-4BFE-BF7B-0F10E9422423}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -36490,23 +37765,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1F713C-62A2-4946-B10B-F5C365A7F2BC}">
-  <dimension ref="A1:D182"/>
+  <dimension ref="A1:K182"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>251</v>
       </c>
       <c r="C1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>257</v>
+      </c>
+      <c r="K1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>252</v>
       </c>
@@ -36519,8 +37800,14 @@
       <c r="D2">
         <v>534.41700000000003</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="J2">
+        <v>17008.357</v>
+      </c>
+      <c r="K2">
+        <v>6576.723</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>253</v>
       </c>
@@ -36533,8 +37820,14 @@
       <c r="D3">
         <v>553.30100000000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <v>17008.357</v>
+      </c>
+      <c r="K3">
+        <v>6576.723</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>168</v>
       </c>
@@ -36547,8 +37840,14 @@
       <c r="D4">
         <v>570.625</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="J4">
+        <v>14161.092000000001</v>
+      </c>
+      <c r="K4">
+        <v>6359.6170000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>254</v>
       </c>
@@ -36561,8 +37860,14 @@
       <c r="D5">
         <v>575.90899999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="J5">
+        <v>14103.118</v>
+      </c>
+      <c r="K5">
+        <v>6397.125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>255</v>
       </c>
@@ -36575,424 +37880,742 @@
       <c r="D6">
         <v>604.35199999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="J6">
+        <v>14036.084999999999</v>
+      </c>
+      <c r="K6">
+        <v>6367.8289999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>40.561999999999998</v>
       </c>
       <c r="D7">
         <v>574.01300000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <v>17533.687000000002</v>
+      </c>
+      <c r="K7">
+        <v>6823.0739999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>40.417999999999999</v>
       </c>
       <c r="D8">
         <v>590.79100000000005</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <v>14550.880999999999</v>
+      </c>
+      <c r="K8">
+        <v>6361.7079999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>42.695</v>
       </c>
       <c r="D9">
         <v>557.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="J9">
+        <v>14442.607</v>
+      </c>
+      <c r="K9">
+        <v>6382.0640000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>41.470999999999997</v>
       </c>
       <c r="D10">
         <v>543.19100000000003</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <v>14359.975</v>
+      </c>
+      <c r="K10">
+        <v>6878.5410000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>40.545000000000002</v>
       </c>
       <c r="D11">
         <v>564.30100000000004</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="J11">
+        <v>14352.181</v>
+      </c>
+      <c r="K11">
+        <v>7486.1480000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>41.628999999999998</v>
       </c>
       <c r="D12">
         <v>547.78300000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="J12">
+        <v>14355.665000000001</v>
+      </c>
+      <c r="K12">
+        <v>6651.9219999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>40.792999999999999</v>
       </c>
       <c r="D13">
         <v>601.41999999999996</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="J13">
+        <v>14352.77</v>
+      </c>
+      <c r="K13">
+        <v>6371.2550000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>41.140999999999998</v>
       </c>
       <c r="D14">
         <v>551.59100000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <v>14343.445</v>
+      </c>
+      <c r="K14">
+        <v>7285.5349999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>40.853000000000002</v>
       </c>
       <c r="D15">
         <v>603.65700000000004</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="J15">
+        <v>14324.89</v>
+      </c>
+      <c r="K15">
+        <v>7074.08</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C16">
         <v>41.249000000000002</v>
       </c>
       <c r="D16">
         <v>561.28499999999997</v>
       </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J16">
+        <v>14323.895</v>
+      </c>
+      <c r="K16">
+        <v>7392.4870000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>40.15</v>
       </c>
       <c r="D17">
         <v>583.56899999999996</v>
       </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J17">
+        <v>14305.71</v>
+      </c>
+      <c r="K17">
+        <v>7179.8469999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C18">
         <v>40.604999999999997</v>
       </c>
       <c r="D18">
         <v>571.88900000000001</v>
       </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J18">
+        <v>14328.205</v>
+      </c>
+      <c r="K18">
+        <v>7235</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C19">
         <v>41.405999999999999</v>
       </c>
       <c r="D19">
         <v>568.37199999999996</v>
       </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J19">
+        <v>14346.89</v>
+      </c>
+      <c r="K19">
+        <v>6876.5959999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C20">
         <v>40.186</v>
       </c>
       <c r="D20">
         <v>591.70799999999997</v>
       </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J20">
+        <v>14311.24</v>
+      </c>
+      <c r="K20">
+        <v>6936.0590000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C21">
         <v>40.031999999999996</v>
       </c>
       <c r="D21">
         <v>571.35</v>
       </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J21">
+        <v>14354.678</v>
+      </c>
+      <c r="K21">
+        <v>7358.3540000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>40.118000000000002</v>
       </c>
       <c r="D22">
         <v>581.71699999999998</v>
       </c>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J22">
+        <v>14350.985000000001</v>
+      </c>
+      <c r="K22">
+        <v>7432.9210000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C23">
         <v>40.542999999999999</v>
       </c>
       <c r="D23">
         <v>602.45799999999997</v>
       </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J23">
+        <v>14333.406999999999</v>
+      </c>
+      <c r="K23">
+        <v>7577.942</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>40.31</v>
       </c>
       <c r="D24">
         <v>568.11099999999999</v>
       </c>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J24">
+        <v>14323.518</v>
+      </c>
+      <c r="K24">
+        <v>7196.3890000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C25">
         <v>40.576000000000001</v>
       </c>
       <c r="D25">
         <v>559.63199999999995</v>
       </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J25">
+        <v>14366.231</v>
+      </c>
+      <c r="K25">
+        <v>7612.91</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C26">
         <v>40.484000000000002</v>
       </c>
       <c r="D26">
         <v>568.94200000000001</v>
       </c>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J26">
+        <v>14311.763999999999</v>
+      </c>
+      <c r="K26">
+        <v>7526.3580000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C27">
         <v>39.825000000000003</v>
       </c>
       <c r="D27">
         <v>581.65599999999995</v>
       </c>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J27">
+        <v>14310.839</v>
+      </c>
+      <c r="K27">
+        <v>7057.5540000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>39.895000000000003</v>
       </c>
       <c r="D28">
         <v>568.54999999999995</v>
       </c>
-    </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J28">
+        <v>14356.501</v>
+      </c>
+      <c r="K28">
+        <v>7526.0140000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C29">
         <v>41.228000000000002</v>
       </c>
       <c r="D29">
         <v>591.74300000000005</v>
       </c>
-    </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J29">
+        <v>14364.191999999999</v>
+      </c>
+      <c r="K29">
+        <v>7690.7139999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C30">
         <v>39.950000000000003</v>
       </c>
       <c r="D30">
         <v>588.23400000000004</v>
       </c>
-    </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J30">
+        <v>14295.773999999999</v>
+      </c>
+      <c r="K30">
+        <v>7817.652</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C31">
         <v>40.1</v>
       </c>
       <c r="D31">
         <v>570.798</v>
       </c>
-    </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J31">
+        <v>14345.221</v>
+      </c>
+      <c r="K31">
+        <v>7071.1419999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C32">
         <v>40.438000000000002</v>
       </c>
       <c r="D32">
         <v>593.68200000000002</v>
       </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J32">
+        <v>14330.42</v>
+      </c>
+      <c r="K32">
+        <v>6947.5169999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C33">
         <v>40.042999999999999</v>
       </c>
       <c r="D33">
         <v>576.596</v>
       </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J33">
+        <v>14342.254000000001</v>
+      </c>
+      <c r="K33">
+        <v>7341.7830000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C34">
         <v>40.454999999999998</v>
       </c>
       <c r="D34">
         <v>558.43499999999995</v>
       </c>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J34">
+        <v>14347.834999999999</v>
+      </c>
+      <c r="K34">
+        <v>7651.1719999999996</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C35">
         <v>39.975999999999999</v>
       </c>
       <c r="D35">
         <v>566.41399999999999</v>
       </c>
-    </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J35">
+        <v>14371.05</v>
+      </c>
+      <c r="K35">
+        <v>7440.4610000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C36">
         <v>39.892000000000003</v>
       </c>
       <c r="D36">
         <v>576.80700000000002</v>
       </c>
-    </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J36">
+        <v>14346.045</v>
+      </c>
+      <c r="K36">
+        <v>7665.1419999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C37">
         <v>40.570999999999998</v>
       </c>
       <c r="D37">
         <v>569.89700000000005</v>
       </c>
-    </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J37">
+        <v>14329.776</v>
+      </c>
+      <c r="K37">
+        <v>7113.6210000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C38">
         <v>39.81</v>
       </c>
       <c r="D38">
         <v>574.74099999999999</v>
       </c>
-    </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J38">
+        <v>14357.947</v>
+      </c>
+      <c r="K38">
+        <v>6855.1970000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C39">
         <v>40.570999999999998</v>
       </c>
       <c r="D39">
         <v>556.55999999999995</v>
       </c>
-    </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J39">
+        <v>14319.233</v>
+      </c>
+      <c r="K39">
+        <v>7865.9110000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C40">
         <v>39.692999999999998</v>
       </c>
       <c r="D40">
         <v>565.90499999999997</v>
       </c>
-    </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J40">
+        <v>14324.21</v>
+      </c>
+      <c r="K40">
+        <v>7765.1120000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C41">
         <v>40.082000000000001</v>
       </c>
       <c r="D41">
         <v>559.89</v>
       </c>
-    </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J41">
+        <v>14338.620999999999</v>
+      </c>
+      <c r="K41">
+        <v>7216.8320000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C42">
         <v>40.328000000000003</v>
       </c>
       <c r="D42">
         <v>562.62400000000002</v>
       </c>
-    </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J42">
+        <v>14359.984</v>
+      </c>
+      <c r="K42">
+        <v>7376.0510000000004</v>
+      </c>
+    </row>
+    <row r="43" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C43">
         <v>39.798000000000002</v>
       </c>
       <c r="D43">
         <v>578.67499999999995</v>
       </c>
-    </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J43">
+        <v>14328.364</v>
+      </c>
+      <c r="K43">
+        <v>7636.0349999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C44">
         <v>40.787999999999997</v>
       </c>
       <c r="D44">
         <v>562.67100000000005</v>
       </c>
-    </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J44">
+        <v>14335.414000000001</v>
+      </c>
+      <c r="K44">
+        <v>7964.1319999999996</v>
+      </c>
+    </row>
+    <row r="45" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C45">
         <v>40.097999999999999</v>
       </c>
       <c r="D45">
         <v>585.20699999999999</v>
       </c>
-    </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J45">
+        <v>14363.214</v>
+      </c>
+      <c r="K45">
+        <v>7972.9549999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C46">
         <v>40.4</v>
       </c>
       <c r="D46">
         <v>562.14099999999996</v>
       </c>
-    </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J46">
+        <v>14335.397999999999</v>
+      </c>
+      <c r="K46">
+        <v>7660.7330000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C47">
         <v>39.646000000000001</v>
       </c>
       <c r="D47">
         <v>581.72900000000004</v>
       </c>
-    </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J47">
+        <v>14354.882</v>
+      </c>
+      <c r="K47">
+        <v>7428.7669999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C48">
         <v>39.750999999999998</v>
       </c>
       <c r="D48">
         <v>573.32299999999998</v>
       </c>
-    </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J48">
+        <v>14328.598</v>
+      </c>
+      <c r="K48">
+        <v>6663.5420000000004</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C49">
         <v>40.061999999999998</v>
       </c>
       <c r="D49">
         <v>580.87800000000004</v>
       </c>
-    </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J49">
+        <v>14343.97</v>
+      </c>
+      <c r="K49">
+        <v>7677.2169999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C50">
         <v>39.74</v>
       </c>
       <c r="D50">
         <v>580.678</v>
       </c>
-    </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J50">
+        <v>14338.165000000001</v>
+      </c>
+      <c r="K50">
+        <v>7160.37</v>
+      </c>
+    </row>
+    <row r="51" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C51">
         <v>40.104999999999997</v>
       </c>
       <c r="D51">
         <v>580.245</v>
       </c>
-    </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J51">
+        <v>14337.576999999999</v>
+      </c>
+      <c r="K51">
+        <v>7375.1210000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C52">
         <v>40.44</v>
       </c>
       <c r="D52">
         <v>590.05200000000002</v>
       </c>
-    </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J52">
+        <v>14365.184999999999</v>
+      </c>
+      <c r="K52">
+        <v>7095.183</v>
+      </c>
+    </row>
+    <row r="53" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C53">
         <v>40.344000000000001</v>
       </c>
       <c r="D53">
         <v>583.18299999999999</v>
       </c>
-    </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J53">
+        <v>14367.597</v>
+      </c>
+      <c r="K53">
+        <v>7485.6679999999997</v>
+      </c>
+    </row>
+    <row r="54" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C54">
         <v>39.96</v>
       </c>
       <c r="D54">
         <v>578.94500000000005</v>
       </c>
-    </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J54">
+        <v>14349.745999999999</v>
+      </c>
+      <c r="K54">
+        <v>7416.6549999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C55">
         <v>39.741999999999997</v>
       </c>
       <c r="D55">
         <v>581.39400000000001</v>
       </c>
-    </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J55">
+        <v>14323.002</v>
+      </c>
+      <c r="K55">
+        <v>6728.94</v>
+      </c>
+    </row>
+    <row r="56" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C56">
         <v>40.182000000000002</v>
       </c>
       <c r="D56">
         <v>590.76</v>
       </c>
-    </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J56">
+        <v>14368.772999999999</v>
+      </c>
+      <c r="K56">
+        <v>6987.2730000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C57">
         <v>39.767000000000003</v>
       </c>
       <c r="D57">
         <v>570.47699999999998</v>
       </c>
-    </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J57">
+        <v>14379.208000000001</v>
+      </c>
+      <c r="K57">
+        <v>7320.6679999999997</v>
+      </c>
+    </row>
+    <row r="58" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C58">
         <v>40.258000000000003</v>
       </c>
       <c r="D58">
         <v>588.00699999999995</v>
       </c>
-    </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="J58">
+        <v>14364.629000000001</v>
+      </c>
+      <c r="K58">
+        <v>7192.5320000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C59">
         <v>39.804000000000002</v>
       </c>
@@ -37000,7 +38623,7 @@
         <v>577.91899999999998</v>
       </c>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C60">
         <v>40.113</v>
       </c>
@@ -37008,7 +38631,7 @@
         <v>570.28</v>
       </c>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C61">
         <v>40.334000000000003</v>
       </c>
@@ -37016,7 +38639,7 @@
         <v>565.11400000000003</v>
       </c>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C62">
         <v>39.584000000000003</v>
       </c>
@@ -37024,7 +38647,7 @@
         <v>580.90499999999997</v>
       </c>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C63">
         <v>39.604999999999997</v>
       </c>
@@ -37032,7 +38655,7 @@
         <v>572.39200000000005</v>
       </c>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C64">
         <v>40.155999999999999</v>
       </c>

</xml_diff>